<commit_message>
insert section rstudio server
</commit_message>
<xml_diff>
--- a/keyShort.xlsx
+++ b/keyShort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kschool\shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EBF293E-E8FA-435A-BAFC-7E68C0BBC85B}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5184069A-7D4E-4855-B0E1-B7E92A1B81EE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="18075" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="379">
   <si>
     <t>Console</t>
   </si>
@@ -1253,6 +1253,9 @@
   </si>
   <si>
     <t>Command all splits</t>
+  </si>
+  <si>
+    <t>Ctrl+Shift+R/Ctrl+F12</t>
   </si>
 </sst>
 </file>
@@ -18663,8 +18666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IV37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -18672,7 +18675,7 @@
     <col min="1" max="1" width="17.28515625" style="37" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="37" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" style="37" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" style="37" customWidth="1"/>
+    <col min="4" max="4" width="21.140625" style="37" customWidth="1"/>
     <col min="5" max="6" width="18.42578125" style="37" customWidth="1"/>
     <col min="7" max="7" width="16.42578125" style="37" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" style="37" customWidth="1"/>
@@ -18741,7 +18744,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="45" t="s">
-        <v>12</v>
+        <v>378</v>
       </c>
       <c r="E4" s="44" t="s">
         <v>89</v>

</xml_diff>

<commit_message>
Org files added: 2016 and 2017
</commit_message>
<xml_diff>
--- a/keyShort.xlsx
+++ b/keyShort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kschool\shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{667A5D0E-7DFC-4021-BA38-B004D3A23331}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5194FE2-DE2B-4080-8384-DC9D822772C1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="6360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="241">
   <si>
     <t>Navigate Forward</t>
   </si>
@@ -567,12 +567,6 @@
     <t>Display all open buffers</t>
   </si>
   <si>
-    <t xml:space="preserve">C-x C-c </t>
-  </si>
-  <si>
-    <t>Exits Emacs</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-g </t>
   </si>
   <si>
@@ -814,12 +808,6 @@
   </si>
   <si>
     <t>wide / narrow window (^ larger)</t>
-  </si>
-  <si>
-    <t>menu/next/prev/back</t>
-  </si>
-  <si>
-    <t>m/n/p/back</t>
   </si>
   <si>
     <t xml:space="preserve">C-M-&lt;SPC&gt;/C-M-@ </t>
@@ -881,6 +869,36 @@
   </si>
   <si>
     <t>C-x i</t>
+  </si>
+  <si>
+    <t>m/n/p/u/back</t>
+  </si>
+  <si>
+    <t>menu/next/prev/up/back</t>
+  </si>
+  <si>
+    <t>C-x g</t>
+  </si>
+  <si>
+    <t>Magit status1</t>
+  </si>
+  <si>
+    <t>C-c [</t>
+  </si>
+  <si>
+    <t>add Org file to agenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-c . </t>
+  </si>
+  <si>
+    <t>add task to calendar</t>
+  </si>
+  <si>
+    <t>C-a C-e</t>
+  </si>
+  <si>
+    <t>Export agenda</t>
   </si>
 </sst>
 </file>
@@ -2534,7 +2552,7 @@
   <dimension ref="A2:IV225"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D25" sqref="A1:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2551,30 +2569,30 @@
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2582,13 +2600,13 @@
         <v>140</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2599,10 +2617,10 @@
         <v>142</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2613,10 +2631,10 @@
         <v>144</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2627,24 +2645,24 @@
         <v>146</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>159</v>
+        <v>222</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>160</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>147</v>
+        <v>163</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2655,10 +2673,10 @@
         <v>166</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2669,32 +2687,32 @@
         <v>168</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>169</v>
       </c>
-      <c r="B12" s="18" t="s">
-        <v>170</v>
-      </c>
       <c r="C12" s="18" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>180</v>
+        <v>224</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>176</v>
@@ -2705,86 +2723,86 @@
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>228</v>
+        <v>171</v>
       </c>
       <c r="B14" s="18" t="s">
         <v>172</v>
       </c>
       <c r="C14" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="D14" s="18" t="s">
         <v>175</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" s="19" t="s">
         <v>173</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>174</v>
-      </c>
-      <c r="C15" s="19" t="s">
-        <v>186</v>
-      </c>
       <c r="D15" s="19" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>207</v>
+        <v>188</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B18" s="18" t="s">
         <v>190</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>192</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>195</v>
-      </c>
-      <c r="D19" s="19" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2792,77 +2810,98 @@
         <v>217</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>220</v>
+        <v>203</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>222</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="C22" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="D23" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19"/>
-      <c r="C23" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="D23" s="19" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>213</v>
+        <v>233</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>214</v>
+        <v>234</v>
       </c>
       <c r="C24" s="18" t="s">
-        <v>215</v>
+        <v>235</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>216</v>
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="14"/>
+      <c r="A25" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="19" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="19" t="s">
-        <v>198</v>
-      </c>
       <c r="C29" s="17" t="s">
-        <v>199</v>
-      </c>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A101" s="5"/>
+      <c r="B101" s="6"/>
     </row>
     <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="5"/>
@@ -3725,16 +3764,14 @@
       <c r="D224" s="6"/>
       <c r="E224" s="6"/>
     </row>
-    <row r="225" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="5"/>
-      <c r="B225" s="6"/>
+    <row r="225" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C225" s="6"/>
       <c r="D225" s="6"/>
       <c r="E225" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A14" r:id="rId1" display="C-M-@ " xr:uid="{480A0750-6164-460E-8A84-EF622B39FC99}"/>
+    <hyperlink ref="A13" r:id="rId1" display="C-M-@ " xr:uid="{480A0750-6164-460E-8A84-EF622B39FC99}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>
@@ -3761,38 +3798,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>208</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>210</v>
       </c>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="D3" s="21" t="s">
         <v>214</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>215</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -3911,8 +3948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:IV26"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4721,18 +4758,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
keyshort and 2018 todo list
Signed-off-by: Jose <vera.josemanuel@gmail.com>
</commit_message>
<xml_diff>
--- a/keyShort.xlsx
+++ b/keyShort.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kschool\shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEBFDC9A-5FAD-4CFF-B448-745E062ECD3B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD25AD0F-1F9A-4493-B7A6-D1CB1B58381D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="6360" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="247">
   <si>
     <t>Navigate Forward</t>
   </si>
@@ -546,9 +546,6 @@
     <t>menu</t>
   </si>
   <si>
-    <t>C-x C-s</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-x b </t>
   </si>
   <si>
@@ -558,15 +555,9 @@
     <t xml:space="preserve">C-x k </t>
   </si>
   <si>
-    <t>Kill (close) a buffer</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-x C-b </t>
   </si>
   <si>
-    <t>Display all open buffers</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-g </t>
   </si>
   <si>
@@ -576,15 +567,9 @@
     <t xml:space="preserve">C-x 0 </t>
   </si>
   <si>
-    <t>Deletes the active window</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-x 1 </t>
   </si>
   <si>
-    <t>Deletes other windows</t>
-  </si>
-  <si>
     <t>C-x 2</t>
   </si>
   <si>
@@ -606,66 +591,30 @@
     <t xml:space="preserve">C-x 4 C-f </t>
   </si>
   <si>
-    <t>Finds a file in the other window</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-x 4 0 </t>
   </si>
   <si>
-    <t>Kills the buffer and window</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-M-f </t>
   </si>
   <si>
-    <t>Move forward by s-expression</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-M-b </t>
   </si>
   <si>
-    <t>Move backward by s-expression</t>
-  </si>
-  <si>
     <t xml:space="preserve">M-h </t>
   </si>
   <si>
-    <t>Marks the next paragraph</t>
-  </si>
-  <si>
-    <t>Marks the whole buffer</t>
-  </si>
-  <si>
-    <t>Marks the next s-expression</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C-&lt;SPC&gt;, C-g </t>
-  </si>
-  <si>
-    <t>Deactivates the region</t>
-  </si>
-  <si>
     <t xml:space="preserve">M-x grep </t>
   </si>
   <si>
     <t xml:space="preserve">C-M-s </t>
   </si>
   <si>
-    <t>Begins a regexp incremental search</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-s </t>
   </si>
   <si>
-    <t>Begins an incremental search</t>
-  </si>
-  <si>
     <t>C-x h</t>
   </si>
   <si>
-    <t>Prompts for arguments to grep</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-w </t>
   </si>
   <si>
@@ -696,13 +645,7 @@
     <t>C-x r b</t>
   </si>
   <si>
-    <t>jump to a bookmark</t>
-  </si>
-  <si>
     <t>C-x r l</t>
-  </si>
-  <si>
-    <t>list your bookmarks</t>
   </si>
   <si>
     <t xml:space="preserve">M-x </t>
@@ -750,12 +693,6 @@
     <t>C-c a</t>
   </si>
   <si>
-    <t>Kill active region - cut</t>
-  </si>
-  <si>
-    <t>Copy to kill ring - copy</t>
-  </si>
-  <si>
     <t>Alt + Number</t>
   </si>
   <si>
@@ -783,12 +720,6 @@
     <t>Kill selected</t>
   </si>
   <si>
-    <t>C-x u</t>
-  </si>
-  <si>
-    <t>undo last change</t>
-  </si>
-  <si>
     <t>C-x C-b</t>
   </si>
   <si>
@@ -807,14 +738,101 @@
     <t>C-x { }</t>
   </si>
   <si>
-    <t>wide / narrow window (^ larger)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C-M-&lt;SPC&gt;/C-M-@ </t>
+    <t>C-x C-v</t>
+  </si>
+  <si>
+    <t>Insert content into buffer</t>
+  </si>
+  <si>
+    <t>C-x i</t>
+  </si>
+  <si>
+    <t>m/n/p/u/back</t>
+  </si>
+  <si>
+    <t>menu/next/prev/up/back</t>
+  </si>
+  <si>
+    <t>C-x g</t>
+  </si>
+  <si>
+    <t>Magit status1</t>
+  </si>
+  <si>
+    <t>C-c [</t>
+  </si>
+  <si>
+    <t>add Org file to agenda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C-c . </t>
+  </si>
+  <si>
+    <t>add task to calendar</t>
+  </si>
+  <si>
+    <t>C-a C-e</t>
+  </si>
+  <si>
+    <t>Export agenda</t>
+  </si>
+  <si>
+    <t>C-c h</t>
+  </si>
+  <si>
+    <t>from helm-find-files session</t>
+  </si>
+  <si>
+    <t>s - u - c</t>
+  </si>
+  <si>
+    <t>Stage - Unstage - Commit</t>
+  </si>
+  <si>
+    <t>C-c C-c</t>
+  </si>
+  <si>
+    <t>Commit</t>
+  </si>
+  <si>
+    <t>P - p</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Replace bufffer contents</t>
+  </si>
+  <si>
+    <t>C-x C-w</t>
+  </si>
+  <si>
+    <t>save as</t>
+  </si>
+  <si>
+    <t>Kill a buffer</t>
+  </si>
+  <si>
+    <t>show all open buffers</t>
+  </si>
+  <si>
+    <t>forward s-expression</t>
+  </si>
+  <si>
+    <t>backward s-expression</t>
+  </si>
+  <si>
+    <t>Kill region - cut</t>
+  </si>
+  <si>
+    <t>to kill ring - copy</t>
+  </si>
+  <si>
+    <t>jump to bookmark</t>
   </si>
   <si>
     <r>
-      <t xml:space="preserve">list buffers </t>
+      <t xml:space="preserve">list  </t>
     </r>
     <r>
       <rPr>
@@ -856,73 +874,49 @@
     </r>
   </si>
   <si>
-    <t>Save buffer C-x C-w save as</t>
-  </si>
-  <si>
-    <t>C-x C-v</t>
-  </si>
-  <si>
-    <t>Replace buffer contents</t>
-  </si>
-  <si>
-    <t>Insert content into buffer</t>
-  </si>
-  <si>
-    <t>C-x i</t>
-  </si>
-  <si>
-    <t>m/n/p/u/back</t>
-  </si>
-  <si>
-    <t>menu/next/prev/up/back</t>
-  </si>
-  <si>
-    <t>C-x g</t>
-  </si>
-  <si>
-    <t>Magit status1</t>
-  </si>
-  <si>
-    <t>C-c [</t>
-  </si>
-  <si>
-    <t>add Org file to agenda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C-c . </t>
-  </si>
-  <si>
-    <t>add task to calendar</t>
-  </si>
-  <si>
-    <t>C-a C-e</t>
-  </si>
-  <si>
-    <t>Export agenda</t>
-  </si>
-  <si>
-    <t>C-c h</t>
-  </si>
-  <si>
-    <t>from helm-find-files session</t>
-  </si>
-  <si>
-    <t>s - u - c</t>
-  </si>
-  <si>
-    <t>Stage - Unstage - Commit</t>
-  </si>
-  <si>
-    <t>C-c C-c</t>
-  </si>
-  <si>
-    <t>Commit</t>
-  </si>
-  <si>
-    <t>P - p</t>
-  </si>
-  <si>
-    <t>Push</t>
+    <t>C-M-&lt;SPC&gt;</t>
+  </si>
+  <si>
+    <t>Deactivates region C-g</t>
+  </si>
+  <si>
+    <t>C-&lt;SPC&gt;</t>
+  </si>
+  <si>
+    <t>Mark next paragraph</t>
+  </si>
+  <si>
+    <t>Mark whole buffer</t>
+  </si>
+  <si>
+    <t>Mark next s-expression C-M-@</t>
+  </si>
+  <si>
+    <t>Delete active window</t>
+  </si>
+  <si>
+    <t>Delete other windows</t>
+  </si>
+  <si>
+    <t>file in the other window</t>
+  </si>
+  <si>
+    <t>Kill buffer and window</t>
+  </si>
+  <si>
+    <t>incremental search</t>
+  </si>
+  <si>
+    <t>regexp incremental search</t>
+  </si>
+  <si>
+    <t>arguments to grep</t>
+  </si>
+  <si>
+    <t>list bookmarks</t>
+  </si>
+  <si>
+    <t>wide/narrow (^ larger)</t>
   </si>
 </sst>
 </file>
@@ -2582,17 +2576,17 @@
   <dimension ref="A2:IV221"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="F22" sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="37.85546875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="41.28515625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="34" style="4" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="31" style="4" customWidth="1"/>
     <col min="5" max="5" width="12.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="42.140625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" style="4" customWidth="1"/>
     <col min="7" max="256" width="10.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2601,150 +2595,150 @@
     </row>
     <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="E3" s="19" t="s">
-        <v>203</v>
+        <v>184</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>202</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>230</v>
+        <v>202</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>229</v>
+        <v>201</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>150</v>
+        <v>238</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>235</v>
+        <v>207</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>236</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>140</v>
+        <v>222</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>152</v>
+        <v>239</v>
       </c>
       <c r="E5" s="19" t="s">
-        <v>239</v>
+        <v>211</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>240</v>
+        <v>212</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>142</v>
-      </c>
       <c r="C6" s="18" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>237</v>
+        <v>209</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>238</v>
+        <v>210</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>144</v>
+        <v>224</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>233</v>
+        <v>205</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>146</v>
+        <v>225</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>223</v>
+        <v>246</v>
       </c>
       <c r="E8" s="22" t="s">
-        <v>243</v>
+        <v>215</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>244</v>
+        <v>216</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>164</v>
+        <v>226</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>245</v>
+        <v>217</v>
       </c>
       <c r="F9" s="23" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>166</v>
+        <v>227</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>138</v>
@@ -2753,200 +2747,194 @@
         <v>139</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="F10" s="22" t="s">
-        <v>248</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>168</v>
+        <v>235</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>160</v>
+        <v>240</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>169</v>
+        <v>236</v>
       </c>
       <c r="C12" s="18" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>162</v>
+        <v>241</v>
       </c>
       <c r="E12" s="18"/>
       <c r="F12" s="18"/>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
-        <v>224</v>
+        <v>232</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>170</v>
+        <v>237</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>177</v>
+        <v>242</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
-        <v>171</v>
+        <v>234</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>172</v>
+        <v>233</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>175</v>
+        <v>243</v>
       </c>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
     </row>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>204</v>
+        <v>228</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>179</v>
+        <v>244</v>
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="19"/>
     </row>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>205</v>
+        <v>229</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
     </row>
     <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
-        <v>195</v>
+        <v>176</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>188</v>
+        <v>171</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
       <c r="D17" s="19" t="s">
-        <v>187</v>
+        <v>170</v>
       </c>
       <c r="E17" s="19"/>
       <c r="F17" s="19"/>
     </row>
     <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="18" t="s">
-        <v>189</v>
+        <v>172</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>190</v>
+        <v>230</v>
       </c>
       <c r="C18" s="18" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
-        <v>215</v>
+        <v>194</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>192</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="B20" s="18" t="s">
-        <v>225</v>
+        <v>204</v>
       </c>
       <c r="C20" s="18" t="s">
-        <v>193</v>
+        <v>174</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>232</v>
+        <v>197</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>218</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>220</v>
-      </c>
       <c r="C22" s="18" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2957,12 +2945,12 @@
     </row>
     <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="19" t="s">
-        <v>196</v>
+        <v>177</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="17" t="s">
-        <v>197</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3839,7 +3827,7 @@
   <hyperlinks>
     <hyperlink ref="A13" r:id="rId1" display="C-M-@ " xr:uid="{480A0750-6164-460E-8A84-EF622B39FC99}"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0" right="0" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup orientation="landscape" r:id="rId2"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
@@ -3864,38 +3852,38 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="C1" s="19" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>210</v>
+        <v>189</v>
       </c>
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="21" t="s">
-        <v>211</v>
+        <v>190</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>212</v>
+        <v>191</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="D3" s="21" t="s">
-        <v>214</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -4824,18 +4812,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>199</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>200</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more agenda mode views
</commit_message>
<xml_diff>
--- a/keyShort.xlsx
+++ b/keyShort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kschool\shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89970B13-9B9C-44F2-BC8F-B3E5E4575664}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4117686B-151A-4C3B-8549-180C010C1D95}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="6360" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="6360" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atom" sheetId="6" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="282">
   <si>
     <t>Navigate Forward</t>
   </si>
@@ -742,16 +742,7 @@
     <t>C-c [</t>
   </si>
   <si>
-    <t>add Org file to agenda</t>
-  </si>
-  <si>
     <t xml:space="preserve">C-c . </t>
-  </si>
-  <si>
-    <t>add task to calendar</t>
-  </si>
-  <si>
-    <t>C-a C-e</t>
   </si>
   <si>
     <t>C-c h</t>
@@ -887,9 +878,6 @@
     <t>regexp incremental search</t>
   </si>
   <si>
-    <t>arguments to grep</t>
-  </si>
-  <si>
     <t>list bookmarks</t>
   </si>
   <si>
@@ -959,9 +947,6 @@
     <t>Fold/Unfold all levels</t>
   </si>
   <si>
-    <t>Shift - Tab</t>
-  </si>
-  <si>
     <t>C-c a t</t>
   </si>
   <si>
@@ -977,9 +962,6 @@
     <t>C-c a a</t>
   </si>
   <si>
-    <t>agenda mode (l log display)</t>
-  </si>
-  <si>
     <t>Export menu</t>
   </si>
   <si>
@@ -987,13 +969,79 @@
   </si>
   <si>
     <t>Repeat six times com</t>
+  </si>
+  <si>
+    <t>grep inside files dir</t>
+  </si>
+  <si>
+    <t>Org</t>
+  </si>
+  <si>
+    <t>Magit</t>
+  </si>
+  <si>
+    <t>Shift-Tab</t>
+  </si>
+  <si>
+    <t>C-h t</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Emacs tutorial</t>
+  </si>
+  <si>
+    <t>add Org file to agenda ] to remove</t>
+  </si>
+  <si>
+    <t>add date to tasks</t>
+  </si>
+  <si>
+    <t>add tiem and date to tasks</t>
+  </si>
+  <si>
+    <t>C-u C-c .</t>
+  </si>
+  <si>
+    <t>agenda mode (l log, t todo list)</t>
+  </si>
+  <si>
+    <t>add tag to task</t>
+  </si>
+  <si>
+    <r>
+      <t>C-x C-w</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>agenda view write</t>
+  </si>
+  <si>
+    <t>C-c C-e</t>
+  </si>
+  <si>
+    <t>l log mode, t todo list, A select view</t>
+  </si>
+  <si>
+    <t>v-spc reset views</t>
+  </si>
+  <si>
+    <t>vt-vm-vy views, o delete other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1087,6 +1135,25 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <i/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1178,7 +1245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1212,6 +1279,16 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2379,7 +2456,7 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
@@ -2387,7 +2464,7 @@
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="8" t="s">
         <v>46</v>
       </c>
@@ -2395,7 +2472,7 @@
       <c r="C1" s="8"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="20.25" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>38</v>
       </c>
@@ -2409,7 +2486,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="20.25" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>42</v>
       </c>
@@ -2423,7 +2500,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="20.25" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>47</v>
       </c>
@@ -2437,7 +2514,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="20.25" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>51</v>
       </c>
@@ -2451,7 +2528,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="20.25" customHeight="1">
       <c r="A6" s="19" t="s">
         <v>55</v>
       </c>
@@ -2465,7 +2542,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="20.25" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>59</v>
       </c>
@@ -2477,7 +2554,7 @@
       </c>
       <c r="D7" s="3"/>
     </row>
-    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="20.25" customHeight="1">
       <c r="A8" s="19" t="s">
         <v>62</v>
       </c>
@@ -2491,7 +2568,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="20.25" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>66</v>
       </c>
@@ -2505,7 +2582,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="20.25" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>70</v>
       </c>
@@ -2519,7 +2596,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="20.25" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>74</v>
       </c>
@@ -2543,7 +2620,7 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
     <col min="2" max="2" width="25" customWidth="1"/>
@@ -2551,13 +2628,13 @@
     <col min="4" max="4" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="17.25" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>77</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>79</v>
       </c>
@@ -2565,13 +2642,13 @@
         <v>50</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="17.25" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>80</v>
       </c>
@@ -2585,35 +2662,35 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="17.25" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>81</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>78</v>
       </c>
       <c r="D4" s="19" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.25" customHeight="1">
+      <c r="A5" s="18" t="s">
+        <v>242</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>241</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>245</v>
       </c>
       <c r="C5" s="18" t="s">
         <v>78</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="17.25" customHeight="1">
       <c r="A6" s="19" t="s">
         <v>82</v>
       </c>
@@ -2621,27 +2698,27 @@
         <v>83</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D6" s="19" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="17.25" customHeight="1">
+      <c r="A7" s="18" t="s">
         <v>243</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>247</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>84</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="17.25" customHeight="1">
       <c r="A8" s="19" t="s">
         <v>85</v>
       </c>
@@ -2649,13 +2726,13 @@
         <v>86</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="17.25" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>87</v>
       </c>
@@ -2663,27 +2740,27 @@
         <v>88</v>
       </c>
       <c r="C9" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="17.25" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>250</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="D10" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="D9" s="18" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>254</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>255</v>
-      </c>
-      <c r="C10" s="19" t="s">
-        <v>257</v>
-      </c>
-      <c r="D10" s="19" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" ht="17.25" customHeight="1">
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
     </row>
@@ -2698,10 +2775,10 @@
   <dimension ref="A2:IV221"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="4" customWidth="1"/>
     <col min="2" max="2" width="34" style="4" customWidth="1"/>
@@ -2712,15 +2789,15 @@
     <col min="7" max="256" width="10.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="16"/>
     </row>
-    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="19" t="s">
         <v>193</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>139</v>
@@ -2729,7 +2806,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="18" t="s">
         <v>195</v>
       </c>
@@ -2740,24 +2817,24 @@
         <v>141</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="19" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>142</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="18" t="s">
         <v>135</v>
       </c>
@@ -2771,12 +2848,12 @@
         <v>144</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="19" t="s">
         <v>137</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>145</v>
@@ -2785,26 +2862,26 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="18" t="s">
         <v>138</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="C8" s="18" t="s">
         <v>192</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="19" t="s">
         <v>151</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>147</v>
@@ -2813,12 +2890,12 @@
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="18" t="s">
         <v>152</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C10" s="18" t="s">
         <v>133</v>
@@ -2827,82 +2904,82 @@
         <v>134</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="19" t="s">
         <v>153</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>149</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="18" t="s">
         <v>157</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C12" s="18" t="s">
         <v>150</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="19" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>156</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="18" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C14" s="18" t="s">
         <v>155</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="19" t="s">
         <v>158</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>154</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="18" t="s">
         <v>159</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C16" s="18" t="s">
         <v>162</v>
@@ -2911,7 +2988,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="19" t="s">
         <v>171</v>
       </c>
@@ -2925,12 +3002,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="18" t="s">
         <v>167</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C18" s="18" t="s">
         <v>160</v>
@@ -2939,21 +3016,21 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="19" t="s">
         <v>187</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>168</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="18" t="s">
         <v>196</v>
       </c>
@@ -2967,7 +3044,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15" customHeight="1">
       <c r="A21" s="19" t="s">
         <v>188</v>
       </c>
@@ -2981,12 +3058,12 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15" customHeight="1">
       <c r="A22" s="18" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C22" s="18" t="s">
         <v>185</v>
@@ -2995,7 +3072,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15" customHeight="1">
       <c r="A23" s="19" t="s">
         <v>189</v>
       </c>
@@ -3003,888 +3080,888 @@
         <v>191</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15" customHeight="1">
       <c r="C25" s="17" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15" customHeight="1">
       <c r="B26" s="19" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" ht="15" customHeight="1">
       <c r="A97" s="5"/>
       <c r="B97" s="6"/>
     </row>
-    <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" ht="15" customHeight="1">
       <c r="A98" s="5"/>
       <c r="B98" s="6"/>
       <c r="C98" s="6"/>
       <c r="D98" s="6"/>
       <c r="E98" s="6"/>
     </row>
-    <row r="99" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" ht="15" customHeight="1">
       <c r="A99" s="5"/>
       <c r="B99" s="6"/>
       <c r="C99" s="6"/>
       <c r="D99" s="6"/>
       <c r="E99" s="6"/>
     </row>
-    <row r="100" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" ht="15" customHeight="1">
       <c r="A100" s="5"/>
       <c r="B100" s="6"/>
       <c r="C100" s="6"/>
       <c r="D100" s="6"/>
       <c r="E100" s="6"/>
     </row>
-    <row r="101" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" ht="15" customHeight="1">
       <c r="A101" s="5"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
       <c r="E101" s="6"/>
     </row>
-    <row r="102" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" ht="15" customHeight="1">
       <c r="A102" s="5"/>
       <c r="B102" s="6"/>
       <c r="C102" s="6"/>
       <c r="D102" s="6"/>
       <c r="E102" s="6"/>
     </row>
-    <row r="103" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" ht="15" customHeight="1">
       <c r="A103" s="5"/>
       <c r="B103" s="6"/>
       <c r="C103" s="6"/>
       <c r="D103" s="6"/>
       <c r="E103" s="6"/>
     </row>
-    <row r="104" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" ht="15" customHeight="1">
       <c r="A104" s="5"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>
       <c r="E104" s="6"/>
     </row>
-    <row r="105" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" ht="15" customHeight="1">
       <c r="A105" s="5"/>
       <c r="B105" s="6"/>
       <c r="C105" s="6"/>
       <c r="D105" s="6"/>
       <c r="E105" s="6"/>
     </row>
-    <row r="106" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" ht="15" customHeight="1">
       <c r="A106" s="5"/>
       <c r="B106" s="6"/>
       <c r="C106" s="6"/>
       <c r="D106" s="6"/>
       <c r="E106" s="6"/>
     </row>
-    <row r="107" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" ht="15" customHeight="1">
       <c r="A107" s="5"/>
       <c r="B107" s="6"/>
       <c r="C107" s="6"/>
       <c r="D107" s="6"/>
       <c r="E107" s="6"/>
     </row>
-    <row r="108" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" ht="15" customHeight="1">
       <c r="A108" s="5"/>
       <c r="B108" s="6"/>
       <c r="C108" s="6"/>
       <c r="D108" s="6"/>
       <c r="E108" s="6"/>
     </row>
-    <row r="109" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" ht="15" customHeight="1">
       <c r="A109" s="5"/>
       <c r="B109" s="6"/>
       <c r="C109" s="6"/>
       <c r="D109" s="6"/>
       <c r="E109" s="6"/>
     </row>
-    <row r="110" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" ht="15" customHeight="1">
       <c r="A110" s="5"/>
       <c r="B110" s="6"/>
       <c r="C110" s="6"/>
       <c r="D110" s="6"/>
       <c r="E110" s="6"/>
     </row>
-    <row r="111" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" ht="15" customHeight="1">
       <c r="A111" s="5"/>
       <c r="B111" s="6"/>
       <c r="C111" s="6"/>
       <c r="D111" s="6"/>
       <c r="E111" s="6"/>
     </row>
-    <row r="112" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" ht="15" customHeight="1">
       <c r="A112" s="5"/>
       <c r="B112" s="6"/>
       <c r="C112" s="6"/>
       <c r="D112" s="6"/>
       <c r="E112" s="6"/>
     </row>
-    <row r="113" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="15" customHeight="1">
       <c r="A113" s="5"/>
       <c r="B113" s="6"/>
       <c r="C113" s="6"/>
       <c r="D113" s="6"/>
       <c r="E113" s="6"/>
     </row>
-    <row r="114" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" ht="15" customHeight="1">
       <c r="A114" s="5"/>
       <c r="B114" s="6"/>
       <c r="C114" s="6"/>
       <c r="D114" s="6"/>
       <c r="E114" s="6"/>
     </row>
-    <row r="115" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" ht="15" customHeight="1">
       <c r="A115" s="5"/>
       <c r="B115" s="6"/>
       <c r="C115" s="6"/>
       <c r="D115" s="6"/>
       <c r="E115" s="6"/>
     </row>
-    <row r="116" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" ht="15" customHeight="1">
       <c r="A116" s="5"/>
       <c r="B116" s="6"/>
       <c r="C116" s="6"/>
       <c r="D116" s="6"/>
       <c r="E116" s="6"/>
     </row>
-    <row r="117" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" ht="15" customHeight="1">
       <c r="A117" s="5"/>
       <c r="B117" s="6"/>
       <c r="C117" s="6"/>
       <c r="D117" s="6"/>
       <c r="E117" s="6"/>
     </row>
-    <row r="118" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" ht="15" customHeight="1">
       <c r="A118" s="5"/>
       <c r="B118" s="6"/>
       <c r="C118" s="6"/>
       <c r="D118" s="6"/>
       <c r="E118" s="6"/>
     </row>
-    <row r="119" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="15" customHeight="1">
       <c r="A119" s="5"/>
       <c r="B119" s="6"/>
       <c r="C119" s="6"/>
       <c r="D119" s="6"/>
       <c r="E119" s="6"/>
     </row>
-    <row r="120" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" ht="15" customHeight="1">
       <c r="A120" s="5"/>
       <c r="B120" s="6"/>
       <c r="C120" s="6"/>
       <c r="D120" s="6"/>
       <c r="E120" s="6"/>
     </row>
-    <row r="121" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" ht="15" customHeight="1">
       <c r="A121" s="5"/>
       <c r="B121" s="6"/>
       <c r="C121" s="6"/>
       <c r="D121" s="6"/>
       <c r="E121" s="6"/>
     </row>
-    <row r="122" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="15" customHeight="1">
       <c r="A122" s="5"/>
       <c r="B122" s="6"/>
       <c r="C122" s="6"/>
       <c r="D122" s="6"/>
       <c r="E122" s="6"/>
     </row>
-    <row r="123" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" ht="15" customHeight="1">
       <c r="A123" s="5"/>
       <c r="B123" s="6"/>
       <c r="C123" s="6"/>
       <c r="D123" s="6"/>
       <c r="E123" s="6"/>
     </row>
-    <row r="124" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" ht="15" customHeight="1">
       <c r="A124" s="5"/>
       <c r="B124" s="6"/>
       <c r="C124" s="6"/>
       <c r="D124" s="6"/>
       <c r="E124" s="6"/>
     </row>
-    <row r="125" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" ht="15" customHeight="1">
       <c r="A125" s="5"/>
       <c r="B125" s="6"/>
       <c r="C125" s="6"/>
       <c r="D125" s="6"/>
       <c r="E125" s="6"/>
     </row>
-    <row r="126" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" ht="15" customHeight="1">
       <c r="A126" s="5"/>
       <c r="B126" s="6"/>
       <c r="C126" s="6"/>
       <c r="D126" s="6"/>
       <c r="E126" s="6"/>
     </row>
-    <row r="127" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" ht="15" customHeight="1">
       <c r="A127" s="5"/>
       <c r="B127" s="6"/>
       <c r="C127" s="6"/>
       <c r="D127" s="6"/>
       <c r="E127" s="6"/>
     </row>
-    <row r="128" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:5" ht="15" customHeight="1">
       <c r="A128" s="5"/>
       <c r="B128" s="6"/>
       <c r="C128" s="6"/>
       <c r="D128" s="6"/>
       <c r="E128" s="6"/>
     </row>
-    <row r="129" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" ht="15" customHeight="1">
       <c r="A129" s="5"/>
       <c r="B129" s="6"/>
       <c r="C129" s="6"/>
       <c r="D129" s="6"/>
       <c r="E129" s="6"/>
     </row>
-    <row r="130" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" ht="15" customHeight="1">
       <c r="A130" s="5"/>
       <c r="B130" s="6"/>
       <c r="C130" s="6"/>
       <c r="D130" s="6"/>
       <c r="E130" s="6"/>
     </row>
-    <row r="131" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" ht="15" customHeight="1">
       <c r="A131" s="5"/>
       <c r="B131" s="6"/>
       <c r="C131" s="6"/>
       <c r="D131" s="6"/>
       <c r="E131" s="6"/>
     </row>
-    <row r="132" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" ht="15" customHeight="1">
       <c r="A132" s="5"/>
       <c r="B132" s="6"/>
       <c r="C132" s="6"/>
       <c r="D132" s="6"/>
       <c r="E132" s="6"/>
     </row>
-    <row r="133" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15" customHeight="1">
       <c r="A133" s="5"/>
       <c r="B133" s="6"/>
       <c r="C133" s="6"/>
       <c r="D133" s="6"/>
       <c r="E133" s="6"/>
     </row>
-    <row r="134" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" ht="15" customHeight="1">
       <c r="A134" s="5"/>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
       <c r="D134" s="6"/>
       <c r="E134" s="6"/>
     </row>
-    <row r="135" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" ht="15" customHeight="1">
       <c r="A135" s="5"/>
       <c r="B135" s="6"/>
       <c r="C135" s="6"/>
       <c r="D135" s="6"/>
       <c r="E135" s="6"/>
     </row>
-    <row r="136" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" ht="15" customHeight="1">
       <c r="A136" s="5"/>
       <c r="B136" s="6"/>
       <c r="C136" s="6"/>
       <c r="D136" s="6"/>
       <c r="E136" s="6"/>
     </row>
-    <row r="137" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" ht="15" customHeight="1">
       <c r="A137" s="5"/>
       <c r="B137" s="6"/>
       <c r="C137" s="6"/>
       <c r="D137" s="6"/>
       <c r="E137" s="6"/>
     </row>
-    <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" ht="15" customHeight="1">
       <c r="A138" s="5"/>
       <c r="B138" s="6"/>
       <c r="C138" s="6"/>
       <c r="D138" s="6"/>
       <c r="E138" s="6"/>
     </row>
-    <row r="139" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" ht="15" customHeight="1">
       <c r="A139" s="5"/>
       <c r="B139" s="6"/>
       <c r="C139" s="6"/>
       <c r="D139" s="6"/>
       <c r="E139" s="6"/>
     </row>
-    <row r="140" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" ht="15" customHeight="1">
       <c r="A140" s="5"/>
       <c r="B140" s="6"/>
       <c r="C140" s="6"/>
       <c r="D140" s="6"/>
       <c r="E140" s="6"/>
     </row>
-    <row r="141" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" ht="15" customHeight="1">
       <c r="A141" s="5"/>
       <c r="B141" s="6"/>
       <c r="C141" s="6"/>
       <c r="D141" s="6"/>
       <c r="E141" s="6"/>
     </row>
-    <row r="142" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" ht="15" customHeight="1">
       <c r="A142" s="5"/>
       <c r="B142" s="6"/>
       <c r="C142" s="6"/>
       <c r="D142" s="6"/>
       <c r="E142" s="6"/>
     </row>
-    <row r="143" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" ht="15" customHeight="1">
       <c r="A143" s="5"/>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
       <c r="D143" s="6"/>
       <c r="E143" s="6"/>
     </row>
-    <row r="144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" ht="15" customHeight="1">
       <c r="A144" s="5"/>
       <c r="B144" s="6"/>
       <c r="C144" s="6"/>
       <c r="D144" s="6"/>
       <c r="E144" s="6"/>
     </row>
-    <row r="145" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" ht="15" customHeight="1">
       <c r="A145" s="5"/>
       <c r="B145" s="6"/>
       <c r="C145" s="6"/>
       <c r="D145" s="6"/>
       <c r="E145" s="6"/>
     </row>
-    <row r="146" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:5" ht="15" customHeight="1">
       <c r="A146" s="5"/>
       <c r="B146" s="6"/>
       <c r="C146" s="6"/>
       <c r="D146" s="6"/>
       <c r="E146" s="6"/>
     </row>
-    <row r="147" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:5" ht="15" customHeight="1">
       <c r="A147" s="5"/>
       <c r="B147" s="6"/>
       <c r="C147" s="6"/>
       <c r="D147" s="6"/>
       <c r="E147" s="6"/>
     </row>
-    <row r="148" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:5" ht="15" customHeight="1">
       <c r="A148" s="5"/>
       <c r="B148" s="6"/>
       <c r="C148" s="6"/>
       <c r="D148" s="6"/>
       <c r="E148" s="6"/>
     </row>
-    <row r="149" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" ht="15" customHeight="1">
       <c r="A149" s="5"/>
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
       <c r="D149" s="6"/>
       <c r="E149" s="6"/>
     </row>
-    <row r="150" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:5" ht="15" customHeight="1">
       <c r="A150" s="5"/>
       <c r="B150" s="6"/>
       <c r="C150" s="6"/>
       <c r="D150" s="6"/>
       <c r="E150" s="6"/>
     </row>
-    <row r="151" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:5" ht="15" customHeight="1">
       <c r="A151" s="5"/>
       <c r="B151" s="6"/>
       <c r="C151" s="6"/>
       <c r="D151" s="6"/>
       <c r="E151" s="6"/>
     </row>
-    <row r="152" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:5" ht="15" customHeight="1">
       <c r="A152" s="5"/>
       <c r="B152" s="6"/>
       <c r="C152" s="6"/>
       <c r="D152" s="6"/>
       <c r="E152" s="6"/>
     </row>
-    <row r="153" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:5" ht="15" customHeight="1">
       <c r="A153" s="5"/>
       <c r="B153" s="6"/>
       <c r="C153" s="6"/>
       <c r="D153" s="6"/>
       <c r="E153" s="6"/>
     </row>
-    <row r="154" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:5" ht="15" customHeight="1">
       <c r="A154" s="5"/>
       <c r="B154" s="6"/>
       <c r="C154" s="6"/>
       <c r="D154" s="6"/>
       <c r="E154" s="6"/>
     </row>
-    <row r="155" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:5" ht="15" customHeight="1">
       <c r="A155" s="5"/>
       <c r="B155" s="6"/>
       <c r="C155" s="6"/>
       <c r="D155" s="6"/>
       <c r="E155" s="6"/>
     </row>
-    <row r="156" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:5" ht="15" customHeight="1">
       <c r="A156" s="5"/>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
       <c r="D156" s="6"/>
       <c r="E156" s="6"/>
     </row>
-    <row r="157" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" ht="15" customHeight="1">
       <c r="A157" s="5"/>
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
       <c r="D157" s="6"/>
       <c r="E157" s="6"/>
     </row>
-    <row r="158" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" ht="15" customHeight="1">
       <c r="A158" s="5"/>
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
       <c r="D158" s="6"/>
       <c r="E158" s="6"/>
     </row>
-    <row r="159" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:5" ht="15" customHeight="1">
       <c r="A159" s="5"/>
       <c r="B159" s="6"/>
       <c r="C159" s="6"/>
       <c r="D159" s="6"/>
       <c r="E159" s="6"/>
     </row>
-    <row r="160" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:5" ht="15" customHeight="1">
       <c r="A160" s="5"/>
       <c r="B160" s="6"/>
       <c r="C160" s="6"/>
       <c r="D160" s="6"/>
       <c r="E160" s="6"/>
     </row>
-    <row r="161" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:5" ht="15" customHeight="1">
       <c r="A161" s="5"/>
       <c r="B161" s="6"/>
       <c r="C161" s="6"/>
       <c r="D161" s="6"/>
       <c r="E161" s="6"/>
     </row>
-    <row r="162" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" ht="15" customHeight="1">
       <c r="A162" s="5"/>
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
       <c r="D162" s="6"/>
       <c r="E162" s="6"/>
     </row>
-    <row r="163" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:5" ht="15" customHeight="1">
       <c r="A163" s="5"/>
       <c r="B163" s="6"/>
       <c r="C163" s="6"/>
       <c r="D163" s="6"/>
       <c r="E163" s="6"/>
     </row>
-    <row r="164" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:5" ht="15" customHeight="1">
       <c r="A164" s="5"/>
       <c r="B164" s="6"/>
       <c r="C164" s="6"/>
       <c r="D164" s="6"/>
       <c r="E164" s="6"/>
     </row>
-    <row r="165" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:5" ht="15" customHeight="1">
       <c r="A165" s="5"/>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
       <c r="D165" s="6"/>
       <c r="E165" s="6"/>
     </row>
-    <row r="166" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:5" ht="15" customHeight="1">
       <c r="A166" s="5"/>
       <c r="B166" s="6"/>
       <c r="C166" s="6"/>
       <c r="D166" s="6"/>
       <c r="E166" s="6"/>
     </row>
-    <row r="167" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:5" ht="15" customHeight="1">
       <c r="A167" s="5"/>
       <c r="B167" s="6"/>
       <c r="C167" s="6"/>
       <c r="D167" s="6"/>
       <c r="E167" s="6"/>
     </row>
-    <row r="168" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:5" ht="15" customHeight="1">
       <c r="A168" s="5"/>
       <c r="B168" s="6"/>
       <c r="C168" s="6"/>
       <c r="D168" s="6"/>
       <c r="E168" s="6"/>
     </row>
-    <row r="169" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:5" ht="15" customHeight="1">
       <c r="A169" s="5"/>
       <c r="B169" s="6"/>
       <c r="C169" s="6"/>
       <c r="D169" s="6"/>
       <c r="E169" s="6"/>
     </row>
-    <row r="170" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:5" ht="15" customHeight="1">
       <c r="A170" s="5"/>
       <c r="B170" s="6"/>
       <c r="C170" s="6"/>
       <c r="D170" s="6"/>
       <c r="E170" s="6"/>
     </row>
-    <row r="171" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:5" ht="15" customHeight="1">
       <c r="A171" s="5"/>
       <c r="B171" s="6"/>
       <c r="C171" s="6"/>
       <c r="D171" s="6"/>
       <c r="E171" s="6"/>
     </row>
-    <row r="172" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:5" ht="15" customHeight="1">
       <c r="A172" s="5"/>
       <c r="B172" s="6"/>
       <c r="C172" s="6"/>
       <c r="D172" s="6"/>
       <c r="E172" s="6"/>
     </row>
-    <row r="173" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:5" ht="15" customHeight="1">
       <c r="A173" s="5"/>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="6"/>
       <c r="E173" s="6"/>
     </row>
-    <row r="174" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:5" ht="15" customHeight="1">
       <c r="A174" s="5"/>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
       <c r="E174" s="6"/>
     </row>
-    <row r="175" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:5" ht="15" customHeight="1">
       <c r="A175" s="5"/>
       <c r="B175" s="6"/>
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="E175" s="6"/>
     </row>
-    <row r="176" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:5" ht="15" customHeight="1">
       <c r="A176" s="5"/>
       <c r="B176" s="6"/>
       <c r="C176" s="6"/>
       <c r="D176" s="6"/>
       <c r="E176" s="6"/>
     </row>
-    <row r="177" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:5" ht="15" customHeight="1">
       <c r="A177" s="5"/>
       <c r="B177" s="6"/>
       <c r="C177" s="6"/>
       <c r="D177" s="6"/>
       <c r="E177" s="6"/>
     </row>
-    <row r="178" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:5" ht="15" customHeight="1">
       <c r="A178" s="5"/>
       <c r="B178" s="6"/>
       <c r="C178" s="6"/>
       <c r="D178" s="6"/>
       <c r="E178" s="6"/>
     </row>
-    <row r="179" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:5" ht="15" customHeight="1">
       <c r="A179" s="5"/>
       <c r="B179" s="6"/>
       <c r="C179" s="6"/>
       <c r="D179" s="6"/>
       <c r="E179" s="6"/>
     </row>
-    <row r="180" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:5" ht="15" customHeight="1">
       <c r="A180" s="5"/>
       <c r="B180" s="6"/>
       <c r="C180" s="6"/>
       <c r="D180" s="6"/>
       <c r="E180" s="6"/>
     </row>
-    <row r="181" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:5" ht="15" customHeight="1">
       <c r="A181" s="5"/>
       <c r="B181" s="6"/>
       <c r="C181" s="6"/>
       <c r="D181" s="6"/>
       <c r="E181" s="6"/>
     </row>
-    <row r="182" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:5" ht="15" customHeight="1">
       <c r="A182" s="5"/>
       <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
     </row>
-    <row r="183" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:5" ht="15" customHeight="1">
       <c r="A183" s="5"/>
       <c r="B183" s="6"/>
       <c r="C183" s="6"/>
       <c r="D183" s="6"/>
       <c r="E183" s="6"/>
     </row>
-    <row r="184" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:5" ht="15" customHeight="1">
       <c r="A184" s="5"/>
       <c r="B184" s="6"/>
       <c r="C184" s="6"/>
       <c r="D184" s="6"/>
       <c r="E184" s="6"/>
     </row>
-    <row r="185" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:5" ht="15" customHeight="1">
       <c r="A185" s="5"/>
       <c r="B185" s="6"/>
       <c r="C185" s="6"/>
       <c r="D185" s="6"/>
       <c r="E185" s="6"/>
     </row>
-    <row r="186" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:5" ht="15" customHeight="1">
       <c r="A186" s="5"/>
       <c r="B186" s="6"/>
       <c r="C186" s="6"/>
       <c r="D186" s="6"/>
       <c r="E186" s="6"/>
     </row>
-    <row r="187" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:5" ht="15" customHeight="1">
       <c r="A187" s="5"/>
       <c r="B187" s="6"/>
       <c r="C187" s="6"/>
       <c r="D187" s="6"/>
       <c r="E187" s="6"/>
     </row>
-    <row r="188" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:5" ht="15" customHeight="1">
       <c r="A188" s="5"/>
       <c r="B188" s="6"/>
       <c r="C188" s="6"/>
       <c r="D188" s="6"/>
       <c r="E188" s="6"/>
     </row>
-    <row r="189" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:5" ht="15" customHeight="1">
       <c r="A189" s="5"/>
       <c r="B189" s="6"/>
       <c r="C189" s="6"/>
       <c r="D189" s="6"/>
       <c r="E189" s="6"/>
     </row>
-    <row r="190" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:5" ht="15" customHeight="1">
       <c r="A190" s="5"/>
       <c r="B190" s="6"/>
       <c r="C190" s="6"/>
       <c r="D190" s="6"/>
       <c r="E190" s="6"/>
     </row>
-    <row r="191" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:5" ht="15" customHeight="1">
       <c r="A191" s="5"/>
       <c r="B191" s="6"/>
       <c r="C191" s="6"/>
       <c r="D191" s="6"/>
       <c r="E191" s="6"/>
     </row>
-    <row r="192" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:5" ht="15" customHeight="1">
       <c r="A192" s="5"/>
       <c r="B192" s="6"/>
       <c r="C192" s="6"/>
       <c r="D192" s="6"/>
       <c r="E192" s="6"/>
     </row>
-    <row r="193" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:5" ht="15" customHeight="1">
       <c r="A193" s="5"/>
       <c r="B193" s="6"/>
       <c r="C193" s="6"/>
       <c r="D193" s="6"/>
       <c r="E193" s="6"/>
     </row>
-    <row r="194" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:5" ht="15" customHeight="1">
       <c r="A194" s="5"/>
       <c r="B194" s="6"/>
       <c r="C194" s="6"/>
       <c r="D194" s="6"/>
       <c r="E194" s="6"/>
     </row>
-    <row r="195" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:5" ht="15" customHeight="1">
       <c r="A195" s="5"/>
       <c r="B195" s="6"/>
       <c r="C195" s="6"/>
       <c r="D195" s="6"/>
       <c r="E195" s="6"/>
     </row>
-    <row r="196" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:5" ht="15" customHeight="1">
       <c r="A196" s="5"/>
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
       <c r="D196" s="6"/>
       <c r="E196" s="6"/>
     </row>
-    <row r="197" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:5" ht="15" customHeight="1">
       <c r="A197" s="5"/>
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
       <c r="D197" s="6"/>
       <c r="E197" s="6"/>
     </row>
-    <row r="198" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:5" ht="15" customHeight="1">
       <c r="A198" s="5"/>
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="6"/>
       <c r="E198" s="6"/>
     </row>
-    <row r="199" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:5" ht="15" customHeight="1">
       <c r="A199" s="5"/>
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="6"/>
       <c r="E199" s="6"/>
     </row>
-    <row r="200" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:5" ht="15" customHeight="1">
       <c r="A200" s="5"/>
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="6"/>
       <c r="E200" s="6"/>
     </row>
-    <row r="201" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:5" ht="15" customHeight="1">
       <c r="A201" s="5"/>
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="6"/>
       <c r="E201" s="6"/>
     </row>
-    <row r="202" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:5" ht="15" customHeight="1">
       <c r="A202" s="5"/>
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="6"/>
       <c r="E202" s="6"/>
     </row>
-    <row r="203" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:5" ht="15" customHeight="1">
       <c r="A203" s="5"/>
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="6"/>
       <c r="E203" s="6"/>
     </row>
-    <row r="204" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:5" ht="15" customHeight="1">
       <c r="A204" s="5"/>
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
       <c r="E204" s="6"/>
     </row>
-    <row r="205" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:5" ht="15" customHeight="1">
       <c r="A205" s="5"/>
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="6"/>
       <c r="E205" s="6"/>
     </row>
-    <row r="206" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:5" ht="15" customHeight="1">
       <c r="A206" s="5"/>
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="6"/>
       <c r="E206" s="6"/>
     </row>
-    <row r="207" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:5" ht="15" customHeight="1">
       <c r="A207" s="5"/>
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="6"/>
       <c r="E207" s="6"/>
     </row>
-    <row r="208" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:5" ht="15" customHeight="1">
       <c r="A208" s="5"/>
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="6"/>
       <c r="E208" s="6"/>
     </row>
-    <row r="209" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:5" ht="15" customHeight="1">
       <c r="A209" s="5"/>
       <c r="B209" s="6"/>
       <c r="C209" s="6"/>
       <c r="D209" s="6"/>
       <c r="E209" s="6"/>
     </row>
-    <row r="210" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:5" ht="15" customHeight="1">
       <c r="A210" s="5"/>
       <c r="B210" s="6"/>
       <c r="C210" s="6"/>
       <c r="D210" s="6"/>
       <c r="E210" s="6"/>
     </row>
-    <row r="211" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:5" ht="15" customHeight="1">
       <c r="A211" s="5"/>
       <c r="B211" s="6"/>
       <c r="C211" s="6"/>
       <c r="D211" s="6"/>
       <c r="E211" s="6"/>
     </row>
-    <row r="212" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:5" ht="15" customHeight="1">
       <c r="A212" s="5"/>
       <c r="B212" s="6"/>
       <c r="C212" s="6"/>
       <c r="D212" s="6"/>
       <c r="E212" s="6"/>
     </row>
-    <row r="213" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:5" ht="15" customHeight="1">
       <c r="A213" s="5"/>
       <c r="B213" s="6"/>
       <c r="C213" s="6"/>
       <c r="D213" s="6"/>
       <c r="E213" s="6"/>
     </row>
-    <row r="214" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:5" ht="15" customHeight="1">
       <c r="A214" s="5"/>
       <c r="B214" s="6"/>
       <c r="C214" s="6"/>
       <c r="D214" s="6"/>
       <c r="E214" s="6"/>
     </row>
-    <row r="215" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:5" ht="15" customHeight="1">
       <c r="A215" s="5"/>
       <c r="B215" s="6"/>
       <c r="C215" s="6"/>
       <c r="D215" s="6"/>
       <c r="E215" s="6"/>
     </row>
-    <row r="216" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:5" ht="15" customHeight="1">
       <c r="A216" s="5"/>
       <c r="B216" s="6"/>
       <c r="C216" s="6"/>
       <c r="D216" s="6"/>
       <c r="E216" s="6"/>
     </row>
-    <row r="217" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:5" ht="15" customHeight="1">
       <c r="A217" s="5"/>
       <c r="B217" s="6"/>
       <c r="C217" s="6"/>
       <c r="D217" s="6"/>
       <c r="E217" s="6"/>
     </row>
-    <row r="218" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:5" ht="15" customHeight="1">
       <c r="A218" s="5"/>
       <c r="B218" s="6"/>
       <c r="C218" s="6"/>
       <c r="D218" s="6"/>
       <c r="E218" s="6"/>
     </row>
-    <row r="219" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:5" ht="15" customHeight="1">
       <c r="A219" s="5"/>
       <c r="B219" s="6"/>
       <c r="C219" s="6"/>
       <c r="D219" s="6"/>
       <c r="E219" s="6"/>
     </row>
-    <row r="220" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:5" ht="15" customHeight="1">
       <c r="A220" s="5"/>
       <c r="B220" s="6"/>
       <c r="C220" s="6"/>
       <c r="D220" s="6"/>
       <c r="E220" s="6"/>
     </row>
-    <row r="221" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:5" ht="15" customHeight="1">
       <c r="C221" s="6"/>
       <c r="D221" s="6"/>
       <c r="E221" s="6"/>
@@ -3903,26 +3980,34 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EC396C-36A3-4263-AE8B-A7BFAF2AFAEC}">
-  <dimension ref="A3:D9"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A1" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="13.5" customHeight="1">
       <c r="A3" s="19" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>198</v>
@@ -3931,71 +4016,155 @@
         <v>199</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+    <row r="4" spans="1:4" ht="13.5" customHeight="1">
+      <c r="B4" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="13.5" customHeight="1">
+      <c r="B5" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>206</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="13.5" customHeight="1">
+      <c r="B6" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="D6" s="22" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A7" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B7" s="22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A8" s="23" t="s">
+        <v>278</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A9" s="22" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A10" s="19" t="s">
+        <v>257</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A11" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="D4" s="22" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
-        <v>204</v>
-      </c>
-      <c r="B5" s="23" t="s">
+      <c r="B11" s="22" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A12" s="19" t="s">
+        <v>273</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A13" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A14" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="C5" s="23" t="s">
-        <v>209</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="C6" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>262</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
-        <v>260</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>259</v>
-      </c>
+      <c r="B14" s="23" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A15" s="22" t="s">
+        <v>276</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="13.5" customHeight="1">
+      <c r="A16" s="19" t="s">
+        <v>268</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A17" s="26"/>
+      <c r="B17" s="22"/>
+    </row>
+    <row r="18" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A18" s="25"/>
+    </row>
+    <row r="19" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A19" s="27"/>
+    </row>
+    <row r="21" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A21" s="26"/>
+    </row>
+    <row r="22" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A22" s="25"/>
+    </row>
+    <row r="23" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A23" s="27"/>
+    </row>
+    <row r="25" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A25" s="26"/>
+    </row>
+    <row r="26" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A26" s="26"/>
+    </row>
+    <row r="27" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A27" s="26"/>
+    </row>
+    <row r="28" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A28" s="26"/>
+    </row>
+    <row r="29" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A29" s="26"/>
+    </row>
+    <row r="30" spans="1:2" ht="13.5" customHeight="1">
+      <c r="A30" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4011,14 +4180,14 @@
       <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="19" t="s">
         <v>179</v>
       </c>
@@ -4030,7 +4199,7 @@
       </c>
       <c r="D1" s="19"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="18" t="s">
         <v>181</v>
       </c>
@@ -4040,7 +4209,7 @@
       <c r="C2" s="18"/>
       <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="21" t="s">
         <v>183</v>
       </c>
@@ -4068,19 +4237,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.85546875" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75">
       <c r="A1" s="8" t="s">
         <v>90</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>79</v>
       </c>
@@ -4088,7 +4257,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75">
       <c r="A3" s="18" t="s">
         <v>80</v>
       </c>
@@ -4096,7 +4265,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="19" t="s">
         <v>92</v>
       </c>
@@ -4104,7 +4273,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="18" t="s">
         <v>85</v>
       </c>
@@ -4112,7 +4281,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="19" t="s">
         <v>95</v>
       </c>
@@ -4120,7 +4289,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="18" t="s">
         <v>96</v>
       </c>
@@ -4128,7 +4297,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="19" t="s">
         <v>102</v>
       </c>
@@ -4136,7 +4305,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="18" t="s">
         <v>103</v>
       </c>
@@ -4144,7 +4313,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75">
       <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
@@ -4152,7 +4321,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="18" t="s">
         <v>106</v>
       </c>
@@ -4174,7 +4343,7 @@
       <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="21" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="2" customWidth="1"/>
@@ -4186,7 +4355,7 @@
     <col min="9" max="256" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:256" ht="15.75" customHeight="1">
       <c r="A1" s="20" t="s">
         <v>2</v>
       </c>
@@ -4194,7 +4363,7 @@
       <c r="C1" s="18"/>
       <c r="D1" s="3"/>
     </row>
-    <row r="2" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:256" ht="15.75" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>12</v>
       </c>
@@ -4208,7 +4377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:256" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>10</v>
       </c>
@@ -4222,7 +4391,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:256" ht="15.75" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>14</v>
       </c>
@@ -4236,7 +4405,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:256" ht="15.75" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>30</v>
       </c>
@@ -4250,7 +4419,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:256" ht="15.75" customHeight="1">
       <c r="A6" s="19" t="s">
         <v>16</v>
       </c>
@@ -4264,7 +4433,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="7" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:256" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
         <v>20</v>
       </c>
@@ -4530,7 +4699,7 @@
       <c r="IU7" s="4"/>
       <c r="IV7" s="4"/>
     </row>
-    <row r="8" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:256" ht="15.75" customHeight="1">
       <c r="A8" s="19" t="s">
         <v>34</v>
       </c>
@@ -4544,7 +4713,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:256" ht="15.75" customHeight="1">
       <c r="A9" s="18" t="s">
         <v>22</v>
       </c>
@@ -4558,7 +4727,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:256" ht="15.75" customHeight="1">
       <c r="A10" s="19" t="s">
         <v>3</v>
       </c>
@@ -4824,7 +4993,7 @@
       <c r="IU10" s="4"/>
       <c r="IV10" s="4"/>
     </row>
-    <row r="11" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:256" ht="15.75" customHeight="1">
       <c r="A11" s="18" t="s">
         <v>7</v>
       </c>
@@ -4838,18 +5007,18 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:256" ht="15.75" customHeight="1"/>
+    <row r="13" spans="1:256" ht="16.5" customHeight="1">
       <c r="G13" s="1"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:256" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:256" ht="16.5" customHeight="1">
       <c r="D14" s="9"/>
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:256" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:256" ht="15.75" customHeight="1">
       <c r="C15" s="13" t="s">
         <v>111</v>
       </c>
@@ -4859,7 +5028,7 @@
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:256" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:256" ht="15" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>108</v>
       </c>
@@ -4871,7 +5040,7 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" ht="15" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>109</v>
       </c>
@@ -4884,7 +5053,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15" customHeight="1">
       <c r="A18" s="14" t="s">
         <v>114</v>
       </c>
@@ -4894,34 +5063,34 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15" customHeight="1">
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15" customHeight="1">
       <c r="C22" s="4"/>
       <c r="D22" s="8" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15" customHeight="1">
       <c r="C23" s="4"/>
       <c r="D23" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15" customHeight="1">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15" customHeight="1">
       <c r="B25" s="4"/>
       <c r="E25" s="11" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="14.25" customHeight="1">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
     </row>
@@ -4942,19 +5111,19 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.85546875" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="8" t="s">
         <v>122</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75">
       <c r="A2" s="19" t="s">
         <v>124</v>
       </c>
@@ -4962,7 +5131,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="18" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>125</v>
       </c>
@@ -4970,7 +5139,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="19" t="s">
         <v>127</v>
       </c>
@@ -4978,7 +5147,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -4986,7 +5155,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>176</v>
       </c>
@@ -5003,25 +5172,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99839666-62E0-4D7C-B7FF-6055F88B2EDA}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.28515625" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="14.25" customHeight="1">
       <c r="A1" s="8" t="s">
         <v>99</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="14.25" customHeight="1">
       <c r="A2" s="19" t="s">
         <v>117</v>
       </c>
@@ -5032,7 +5201,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="14.25" customHeight="1">
       <c r="A3" s="18" t="s">
         <v>96</v>
       </c>
@@ -5041,7 +5210,7 @@
       </c>
       <c r="C3" s="18"/>
     </row>
-    <row r="4" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="14.25" customHeight="1">
       <c r="A4" s="19" t="s">
         <v>100</v>
       </c>
@@ -5050,7 +5219,7 @@
       </c>
       <c r="C4" s="19"/>
     </row>
-    <row r="5" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="14.25" customHeight="1">
       <c r="A5" s="18" t="s">
         <v>118</v>
       </c>

</xml_diff>

<commit_message>
por fin byobu keybindings
</commit_message>
<xml_diff>
--- a/keyShort.xlsx
+++ b/keyShort.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\kschool\shortcuts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE13B79A-A716-49A6-9C7C-F6A0CAD4899A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65712E66-5DA6-446A-B3D5-38C4012ABA19}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="6360" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="45" windowWidth="15960" windowHeight="6360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="atom" sheetId="6" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="265">
   <si>
     <t>Navigate Forward</t>
   </si>
@@ -265,12 +265,6 @@
     <t>Split Vertically</t>
   </si>
   <si>
-    <t>Move to Split</t>
-  </si>
-  <si>
-    <t>Detach (no out)</t>
-  </si>
-  <si>
     <t>Shift + F6</t>
   </si>
   <si>
@@ -278,9 +272,6 @@
   </si>
   <si>
     <t>Kill Window/Split</t>
-  </si>
-  <si>
-    <t>Ctrl + F6</t>
   </si>
   <si>
     <t>Rename Window</t>
@@ -674,24 +665,6 @@
     <t>Shift + F1</t>
   </si>
   <si>
-    <t>F3 / F4 - Alt+Cursor</t>
-  </si>
-  <si>
-    <t>Move to session</t>
-  </si>
-  <si>
-    <t>Alt + up/down</t>
-  </si>
-  <si>
-    <t>Alt + left/right</t>
-  </si>
-  <si>
-    <t>Shift + Alt + Cursor</t>
-  </si>
-  <si>
-    <t>Resize Split</t>
-  </si>
-  <si>
     <t>Detach &amp; log out</t>
   </si>
   <si>
@@ -716,16 +689,10 @@
     <t>F12</t>
   </si>
   <si>
-    <t>Escape</t>
-  </si>
-  <si>
     <t>Toggle keybindings</t>
   </si>
   <si>
     <t xml:space="preserve">Shift + F12 </t>
-  </si>
-  <si>
-    <t>Shift + F3/F4</t>
   </si>
   <si>
     <t>Fold/Unfold all levels</t>
@@ -876,6 +843,69 @@
   </si>
   <si>
     <t>Mark region, move cursor</t>
+  </si>
+  <si>
+    <t>Shift + right/left</t>
+  </si>
+  <si>
+    <t>Show numbers</t>
+  </si>
+  <si>
+    <t>Ctrl + D (exit RET)</t>
+  </si>
+  <si>
+    <t>Alt + left/right (F3-F4)</t>
+  </si>
+  <si>
+    <t>Move to Split r/l</t>
+  </si>
+  <si>
+    <t>c  create window</t>
+  </si>
+  <si>
+    <t>w  list windows</t>
+  </si>
+  <si>
+    <t>n  next window</t>
+  </si>
+  <si>
+    <t>p  previous window</t>
+  </si>
+  <si>
+    <t>f  find window</t>
+  </si>
+  <si>
+    <t>,  name window</t>
+  </si>
+  <si>
+    <t>&amp;  kill window</t>
+  </si>
+  <si>
+    <t>| Split horiz</t>
+  </si>
+  <si>
+    <t>% split vert</t>
+  </si>
+  <si>
+    <t>o  swap panes</t>
+  </si>
+  <si>
+    <t>q  show pane numbers</t>
+  </si>
+  <si>
+    <t>k  kill pane</t>
+  </si>
+  <si>
+    <t>d  detach</t>
+  </si>
+  <si>
+    <t>t  big clock</t>
+  </si>
+  <si>
+    <t>?  list shortcuts</t>
+  </si>
+  <si>
+    <t>:  prompt</t>
   </si>
 </sst>
 </file>
@@ -2419,153 +2449,178 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7589D3-2D47-45A7-B18F-F531AE67900B}">
-  <dimension ref="A2:D11"/>
+  <dimension ref="A2:D17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
-    <col min="2" max="2" width="25" customWidth="1"/>
-    <col min="3" max="3" width="19.5703125" customWidth="1"/>
-    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="17.25" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>77</v>
+        <v>248</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>190</v>
+        <v>244</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="17.25" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>78</v>
+        <v>245</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>53</v>
+        <v>256</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17.25" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>79</v>
+        <v>188</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>208</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>191</v>
+        <v>80</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17.25" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>196</v>
+        <v>81</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>76</v>
+        <v>246</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>194</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17.25" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>193</v>
+        <v>83</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="17.25" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>198</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17.25" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>199</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>200</v>
+        <v>53</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>253</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="17.25" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>203</v>
+        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.25" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>207</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>206</v>
+        <v>189</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17.25" customHeight="1">
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
+      <c r="A11" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="17.25" customHeight="1">
+      <c r="A12" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="17.25" customHeight="1">
+      <c r="A13" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B13" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="17.25" customHeight="1">
+      <c r="D14" s="12" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="17.25" customHeight="1">
+      <c r="D15" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="17.25" customHeight="1">
+      <c r="D16" s="12" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" ht="17.25" customHeight="1">
+      <c r="D17" s="12" t="s">
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2590,254 +2645,254 @@
   <sheetData>
     <row r="2" spans="1:4" ht="15" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>118</v>
-      </c>
       <c r="D3" s="12" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="12" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="12" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D10" s="13" t="s">
         <v>180</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>126</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="12" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="13" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="12" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B17" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C17" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>146</v>
-      </c>
       <c r="D17" s="12" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="13" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15" customHeight="1">
       <c r="A19" s="12" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="15" customHeight="1">
@@ -3732,7 +3787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7EC396C-36A3-4263-AE8B-A7BFAF2AFAEC}">
   <dimension ref="A2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:D16"/>
     </sheetView>
   </sheetViews>
@@ -3746,186 +3801,186 @@
   <sheetData>
     <row r="2" spans="1:9" ht="13.5" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F2" s="13" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="13.5" customHeight="1">
       <c r="B3" s="15" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D3" s="15" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="E3" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>234</v>
-      </c>
-      <c r="F3" s="12" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="13.5" customHeight="1">
       <c r="B4" s="15" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="13.5" customHeight="1">
       <c r="B5" s="15" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="13.5" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="13.5" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="E7" s="12" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="13.5" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" ht="13.5" customHeight="1">
       <c r="A9" s="16" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="13.5" customHeight="1">
       <c r="A10" s="15" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="13.5" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="13.5" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="13.5" customHeight="1">
       <c r="A13" s="15" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="13.5" customHeight="1">
       <c r="A14" s="16" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="13.5" customHeight="1">
       <c r="A15" s="15" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="13.5" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="13.5" customHeight="1">
@@ -3986,7 +4041,7 @@
         <v>77</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75">
@@ -3994,55 +4049,55 @@
         <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75">
       <c r="A4" s="13" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75">
       <c r="A5" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75">
       <c r="A6" s="13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75">
       <c r="A7" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75">
       <c r="A8" s="13" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75">
       <c r="A9" s="12" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75">
@@ -4050,12 +4105,12 @@
         <v>9</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75">
       <c r="A11" s="12" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>57</v>
@@ -4144,7 +4199,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:256" ht="15.75" customHeight="1">
@@ -4155,10 +4210,10 @@
         <v>16</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:256" ht="15.75" customHeight="1">
@@ -4743,7 +4798,7 @@
     </row>
     <row r="14" spans="1:256" ht="16.5" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D14" s="8"/>
       <c r="G14" s="1"/>
@@ -4751,10 +4806,10 @@
     </row>
     <row r="15" spans="1:256" ht="15" customHeight="1">
       <c r="A15" s="9" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15" customHeight="1">
@@ -4806,18 +4861,18 @@
     </row>
     <row r="2" spans="1:3" ht="14.25" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="14.25" customHeight="1">
       <c r="A3" s="12" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>40</v>
@@ -4826,19 +4881,19 @@
     </row>
     <row r="4" spans="1:3" ht="14.25" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3" ht="14.25" customHeight="1">
       <c r="A5" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C5" s="12"/>
     </row>

</xml_diff>